<commit_message>
GDD Updated (Listed enemy states)
</commit_message>
<xml_diff>
--- a/Documentation/burndownchart.xlsx
+++ b/Documentation/burndownchart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C++\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375A3D93-1360-42DB-AB71-6DFC45625219}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7316E0B4-53BA-4360-9547-C8FC1101AD36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{5F5C454C-84B7-4EA7-AE0C-67859527ADDE}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,13 +50,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,15 +85,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="2" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -113,11 +136,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -145,11 +168,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -170,8 +193,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Current</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="31750" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -180,8 +214,72 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$19:$M$19</c:f>
@@ -231,8 +329,19 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="31750" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -241,8 +350,72 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$20:$M$20</c:f>
@@ -290,13 +463,15 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1020454143"/>
         <c:axId val="1019796751"/>
@@ -314,11 +489,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -330,11 +505,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -357,17 +532,29 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="95000"/>
+                      <a:lumOff val="5000"/>
+                      <a:alpha val="42000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="36000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -377,33 +564,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="1020454143"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -417,10 +577,15 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -433,9 +598,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -452,14 +617,30 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -525,146 +706,174 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="75000"/>
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="25000"/>
             <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -673,36 +882,29 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -718,21 +920,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -747,13 +947,13 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -766,17 +966,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -785,12 +985,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -804,30 +1004,36 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -837,17 +1043,28 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -856,12 +1073,88 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="75000"/>
             <a:lumOff val="25000"/>
           </a:schemeClr>
@@ -869,64 +1162,6 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -934,14 +1169,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -953,12 +1188,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -967,14 +1202,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -983,9 +1217,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1003,9 +1237,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1016,11 +1250,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1028,14 +1267,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1380,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B264F07D-4A62-4CA4-BDF9-890D6D6CAE75}">
   <dimension ref="A2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1748,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C19">
@@ -1564,7 +1797,7 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="2">

</xml_diff>

<commit_message>
Multithreading integrated, Input and Render processes run on different threads now (Thread object exists within the process.h and its child classes).
</commit_message>
<xml_diff>
--- a/Documentation/burndownchart.xlsx
+++ b/Documentation/burndownchart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C++\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3F19F8-42BC-45C5-BB3A-026B45E3AAAF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9A0A70-21FA-4382-BC13-8A0F6F2A1FDD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{5F5C454C-84B7-4EA7-AE0C-67859527ADDE}"/>
   </bookViews>
@@ -287,7 +287,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10</c:v>
@@ -305,10 +305,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1613,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B264F07D-4A62-4CA4-BDF9-890D6D6CAE75}">
   <dimension ref="A2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,6 +1732,9 @@
         <v>10</v>
       </c>
       <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>3</v>
       </c>
       <c r="G13">
@@ -1744,6 +1747,9 @@
         <v>2</v>
       </c>
       <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>2</v>
       </c>
     </row>
@@ -1787,7 +1793,7 @@
       </c>
       <c r="D19">
         <f>C19-SUM(D5:D16)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E19">
         <f t="shared" ref="E19:M19" si="0">D19-SUM(E5:E16)</f>
@@ -1811,11 +1817,11 @@
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
@@ -1843,7 +1849,7 @@
         <v>12.8</v>
       </c>
       <c r="F20">
-        <f t="shared" ref="F20:M20" si="1">E20-$C$20</f>
+        <f t="shared" ref="F20:L20" si="1">E20-$C$20</f>
         <v>11.200000000000001</v>
       </c>
       <c r="G20">

</xml_diff>

<commit_message>
Vulkan developed until pipeline
</commit_message>
<xml_diff>
--- a/Documentation/burndownchart.xlsx
+++ b/Documentation/burndownchart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C++\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9A0A70-21FA-4382-BC13-8A0F6F2A1FDD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{86BE1D5E-1E08-4BE2-95A0-DCF3DDD44173}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{5F5C454C-84B7-4EA7-AE0C-67859527ADDE}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,12 +31,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Time left</t>
   </si>
   <si>
     <t>Current</t>
+  </si>
+  <si>
+    <t>Command to choose difficulty</t>
+  </si>
+  <si>
+    <t>Higher room count with higher difficulty</t>
+  </si>
+  <si>
+    <t>Infinite room generation</t>
+  </si>
+  <si>
+    <t>Multithreading</t>
+  </si>
+  <si>
+    <t>Thread deletion</t>
+  </si>
+  <si>
+    <t>StateMachine</t>
   </si>
 </sst>
 </file>
@@ -287,31 +306,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -423,31 +442,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>14.4</c:v>
+                  <c:v>27.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.8</c:v>
+                  <c:v>24.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.200000000000001</c:v>
+                  <c:v>21.699999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.6000000000000014</c:v>
+                  <c:v>18.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0000000000000018</c:v>
+                  <c:v>15.499999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.4000000000000021</c:v>
+                  <c:v>12.399999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.8000000000000025</c:v>
+                  <c:v>9.2999999999999954</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.2000000000000024</c:v>
+                  <c:v>6.1999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6000000000000023</c:v>
+                  <c:v>3.0999999999999956</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1277,16 +1296,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>468923</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>103676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>164123</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>179876</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1613,173 +1632,146 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B264F07D-4A62-4CA4-BDF9-890D6D6CAE75}">
   <dimension ref="A2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D2" s="1">
-        <v>43374</v>
+        <v>43387</v>
       </c>
       <c r="E2" s="1">
-        <v>43375</v>
+        <v>43388</v>
       </c>
       <c r="F2" s="1">
-        <v>43376</v>
+        <v>43389</v>
       </c>
       <c r="G2" s="1">
-        <v>43377</v>
+        <v>43390</v>
       </c>
       <c r="H2" s="1">
-        <v>43378</v>
+        <v>43391</v>
       </c>
       <c r="I2" s="1">
-        <v>43381</v>
+        <v>43401</v>
       </c>
       <c r="J2" s="1">
-        <v>43382</v>
+        <v>43402</v>
       </c>
       <c r="K2" s="1">
-        <v>43383</v>
+        <v>43403</v>
       </c>
       <c r="L2" s="1">
-        <v>43384</v>
+        <v>43404</v>
       </c>
       <c r="M2" s="1">
-        <v>43385</v>
+        <v>43405</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1.1000000000000001</v>
+      <c r="A5" t="s">
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1.2</v>
+      <c r="A6" t="s">
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1.3</v>
+      <c r="A7" t="s">
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2.2000000000000002</v>
+      <c r="A8" t="s">
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2.2999999999999998</v>
+      <c r="A9" t="s">
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3.1</v>
+      <c r="A10" t="s">
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>3.2</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3.3</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>3</v>
-      </c>
-      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="I10">
         <v>2</v>
       </c>
-      <c r="H13">
+      <c r="J10">
         <v>2</v>
       </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>4.2</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>5.2</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="D16">
+      <c r="K10">
         <v>1</v>
       </c>
-      <c r="H16">
+      <c r="L10">
         <v>1</v>
       </c>
     </row>
@@ -1789,43 +1781,43 @@
       </c>
       <c r="C19">
         <f>SUM(B5:B16)</f>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D19">
         <f>C19-SUM(D5:D16)</f>
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E19">
         <f t="shared" ref="E19:M19" si="0">D19-SUM(E5:E16)</f>
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M19">
         <f t="shared" si="0"/>
@@ -1838,43 +1830,43 @@
       </c>
       <c r="C20" s="2">
         <f>C19/COUNTA(D2:M2)</f>
-        <v>1.6</v>
+        <v>3.1</v>
       </c>
       <c r="D20">
         <f>C19-C20</f>
-        <v>14.4</v>
+        <v>27.9</v>
       </c>
       <c r="E20">
         <f>D20-$C$20</f>
-        <v>12.8</v>
+        <v>24.799999999999997</v>
       </c>
       <c r="F20">
         <f t="shared" ref="F20:L20" si="1">E20-$C$20</f>
-        <v>11.200000000000001</v>
+        <v>21.699999999999996</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>9.6000000000000014</v>
+        <v>18.599999999999994</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
-        <v>8.0000000000000018</v>
+        <v>15.499999999999995</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
-        <v>6.4000000000000021</v>
+        <v>12.399999999999995</v>
       </c>
       <c r="J20">
         <f t="shared" si="1"/>
-        <v>4.8000000000000025</v>
+        <v>9.2999999999999954</v>
       </c>
       <c r="K20">
         <f t="shared" si="1"/>
-        <v>3.2000000000000024</v>
+        <v>6.1999999999999957</v>
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
-        <v>1.6000000000000023</v>
+        <v>3.0999999999999956</v>
       </c>
       <c r="M20">
         <v>0</v>

</xml_diff>